<commit_message>
Aprimorando sistema para possibilitar concluir cards
</commit_message>
<xml_diff>
--- a/planilha_cards.xlsx
+++ b/planilha_cards.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\141775\Documents\PythonProjects\Automatizacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6660A8B-2E50-4CBC-82B1-6CFC76E0051C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58BD788-8724-4418-8AC1-3E39C4A32A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{65DD3109-69D9-4D8B-AFAF-79D130618933}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Título</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>ENDOMARKETING</t>
+  </si>
+  <si>
+    <t>Baixa</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,6 +474,7 @@
     <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -489,6 +493,9 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -506,6 +513,9 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -540,8 +550,12 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
   </sheetData>

</xml_diff>